<commit_message>
updated for new service
</commit_message>
<xml_diff>
--- a/url_data.xlsx
+++ b/url_data.xlsx
@@ -87,10 +87,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -129,6 +129,16 @@
         <v>8003</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>hystrix-test</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>8004</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
   <printOptions/>

</xml_diff>